<commit_message>
Se crean archivos html para mostrar graficas echas en Python
</commit_message>
<xml_diff>
--- a/data/usuarios_sistema_completo.xlsx
+++ b/data/usuarios_sistema_completo.xlsx
@@ -5283,7 +5283,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5301,12 +5301,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -5353,7 +5347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5373,9 +5367,6 @@
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -5383,7 +5374,7 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5693,14 +5684,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="11.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="30.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="21.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="17.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="18.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="30.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="19.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="8" width="21.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -5818,7 +5809,7 @@
         <v>24</v>
       </c>
       <c r="F5" s="5"/>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <v>20313</v>
       </c>
       <c r="H5" s="5" t="s">
@@ -5868,7 +5859,7 @@
       <c r="F7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>33011</v>
       </c>
       <c r="H7" s="5" t="s">
@@ -5894,7 +5885,7 @@
       <c r="F8" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <v>36356</v>
       </c>
       <c r="H8" s="5" t="s">
@@ -5920,7 +5911,7 @@
       <c r="F9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>20313</v>
       </c>
       <c r="H9" s="5" t="s">
@@ -5968,14 +5959,14 @@
         <v>24</v>
       </c>
       <c r="F11" s="5"/>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <v>21366</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -5999,7 +5990,7 @@
       </c>
       <c r="H12" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -6023,7 +6014,7 @@
       </c>
       <c r="H13" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -6040,14 +6031,14 @@
         <v>24</v>
       </c>
       <c r="F14" s="5"/>
-      <c r="G14" s="7">
+      <c r="G14" s="6">
         <v>23193</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -6071,7 +6062,7 @@
       </c>
       <c r="H15" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -6090,14 +6081,14 @@
       <c r="F16" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="6">
         <v>30571</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -6116,14 +6107,14 @@
       <c r="F17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="6">
         <v>28096</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -6140,14 +6131,14 @@
         <v>24</v>
       </c>
       <c r="F18" s="5"/>
-      <c r="G18" s="7">
+      <c r="G18" s="6">
         <v>29631</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -6166,14 +6157,14 @@
       <c r="F19" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="6">
         <v>20313</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -6197,7 +6188,7 @@
       </c>
       <c r="H20" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -6221,7 +6212,7 @@
       </c>
       <c r="H21" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -6245,7 +6236,7 @@
       </c>
       <c r="H22" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -6269,7 +6260,7 @@
       </c>
       <c r="H23" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -6286,14 +6277,14 @@
         <v>24</v>
       </c>
       <c r="F24" s="5"/>
-      <c r="G24" s="7">
+      <c r="G24" s="6">
         <v>30571</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -6310,7 +6301,7 @@
         <v>24</v>
       </c>
       <c r="F25" s="5"/>
-      <c r="G25" s="7">
+      <c r="G25" s="6">
         <v>32348</v>
       </c>
       <c r="H25" s="5" t="s">
@@ -6334,7 +6325,7 @@
         <v>24</v>
       </c>
       <c r="F26" s="5"/>
-      <c r="G26" s="7">
+      <c r="G26" s="6">
         <v>33011</v>
       </c>
       <c r="H26" s="5" t="s">
@@ -6360,7 +6351,7 @@
       <c r="F27" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="6">
         <v>23509</v>
       </c>
       <c r="H27" s="5" t="s">
@@ -6384,7 +6375,7 @@
         <v>24</v>
       </c>
       <c r="F28" s="5"/>
-      <c r="G28" s="7">
+      <c r="G28" s="6">
         <v>23193</v>
       </c>
       <c r="H28" s="5" t="s">
@@ -6408,7 +6399,7 @@
         <v>24</v>
       </c>
       <c r="F29" s="5"/>
-      <c r="G29" s="7">
+      <c r="G29" s="6">
         <v>27277</v>
       </c>
       <c r="H29" s="5" t="s">
@@ -6456,7 +6447,7 @@
         <v>24</v>
       </c>
       <c r="F31" s="5"/>
-      <c r="G31" s="7">
+      <c r="G31" s="6">
         <v>30571</v>
       </c>
       <c r="H31" s="5" t="s">
@@ -6528,7 +6519,7 @@
         <v>24</v>
       </c>
       <c r="F34" s="5"/>
-      <c r="G34" s="7">
+      <c r="G34" s="6">
         <v>23509</v>
       </c>
       <c r="H34" s="5" t="s">
@@ -6720,7 +6711,7 @@
         <v>24</v>
       </c>
       <c r="F42" s="5"/>
-      <c r="G42" s="7">
+      <c r="G42" s="6">
         <v>32348</v>
       </c>
       <c r="H42" s="5" t="s">
@@ -6816,7 +6807,7 @@
         <v>24</v>
       </c>
       <c r="F46" s="5"/>
-      <c r="G46" s="7">
+      <c r="G46" s="6">
         <v>34367</v>
       </c>
       <c r="H46" s="5" t="s">
@@ -6840,7 +6831,7 @@
         <v>24</v>
       </c>
       <c r="F47" s="5"/>
-      <c r="G47" s="7">
+      <c r="G47" s="6">
         <v>36356</v>
       </c>
       <c r="H47" s="5" t="s">
@@ -6864,7 +6855,7 @@
         <v>24</v>
       </c>
       <c r="F48" s="5"/>
-      <c r="G48" s="7">
+      <c r="G48" s="6">
         <v>35875</v>
       </c>
       <c r="H48" s="5" t="s">
@@ -6888,7 +6879,7 @@
         <v>24</v>
       </c>
       <c r="F49" s="5"/>
-      <c r="G49" s="7">
+      <c r="G49" s="6">
         <v>30571</v>
       </c>
       <c r="H49" s="5" t="s">
@@ -6936,7 +6927,7 @@
         <v>24</v>
       </c>
       <c r="F51" s="5"/>
-      <c r="G51" s="7">
+      <c r="G51" s="6">
         <v>36328</v>
       </c>
       <c r="H51" s="5" t="s">
@@ -6984,7 +6975,7 @@
         <v>24</v>
       </c>
       <c r="F53" s="5"/>
-      <c r="G53" s="7">
+      <c r="G53" s="6">
         <v>23509</v>
       </c>
       <c r="H53" s="5" t="s">
@@ -7010,7 +7001,7 @@
       <c r="F54" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G54" s="7">
+      <c r="G54" s="6">
         <v>21129</v>
       </c>
       <c r="H54" s="5" t="s">
@@ -7034,7 +7025,7 @@
         <v>24</v>
       </c>
       <c r="F55" s="5"/>
-      <c r="G55" s="7">
+      <c r="G55" s="6">
         <v>27277</v>
       </c>
       <c r="H55" s="5" t="s">
@@ -7082,7 +7073,7 @@
         <v>24</v>
       </c>
       <c r="F57" s="5"/>
-      <c r="G57" s="7">
+      <c r="G57" s="6">
         <v>28865</v>
       </c>
       <c r="H57" s="5" t="s">
@@ -7154,7 +7145,7 @@
         <v>24</v>
       </c>
       <c r="F60" s="5"/>
-      <c r="G60" s="7">
+      <c r="G60" s="6">
         <v>30571</v>
       </c>
       <c r="H60" s="5" t="s">
@@ -7226,7 +7217,7 @@
         <v>24</v>
       </c>
       <c r="F63" s="5"/>
-      <c r="G63" s="7">
+      <c r="G63" s="6">
         <v>34367</v>
       </c>
       <c r="H63" s="5" t="s">
@@ -7250,7 +7241,7 @@
         <v>24</v>
       </c>
       <c r="F64" s="5"/>
-      <c r="G64" s="7">
+      <c r="G64" s="6">
         <v>28865</v>
       </c>
       <c r="H64" s="5" t="s">
@@ -7322,7 +7313,7 @@
         <v>24</v>
       </c>
       <c r="F67" s="5"/>
-      <c r="G67" s="7">
+      <c r="G67" s="6">
         <v>35875</v>
       </c>
       <c r="H67" s="5" t="s">
@@ -7346,7 +7337,7 @@
         <v>24</v>
       </c>
       <c r="F68" s="5"/>
-      <c r="G68" s="7">
+      <c r="G68" s="6">
         <v>23193</v>
       </c>
       <c r="H68" s="5" t="s">
@@ -7370,7 +7361,7 @@
         <v>24</v>
       </c>
       <c r="F69" s="5"/>
-      <c r="G69" s="7">
+      <c r="G69" s="6">
         <v>21129</v>
       </c>
       <c r="H69" s="5" t="s">
@@ -7420,7 +7411,7 @@
       <c r="F71" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G71" s="7">
+      <c r="G71" s="6">
         <v>32348</v>
       </c>
       <c r="H71" s="5" t="s">
@@ -7516,7 +7507,7 @@
         <v>24</v>
       </c>
       <c r="F75" s="5"/>
-      <c r="G75" s="7">
+      <c r="G75" s="6">
         <v>24699</v>
       </c>
       <c r="H75" s="5" t="s">
@@ -7566,7 +7557,7 @@
       <c r="F77" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G77" s="7">
+      <c r="G77" s="6">
         <v>26395</v>
       </c>
       <c r="H77" s="5" t="s">
@@ -7614,7 +7605,7 @@
         <v>53</v>
       </c>
       <c r="F79" s="5"/>
-      <c r="G79" s="7">
+      <c r="G79" s="6">
         <v>30191</v>
       </c>
       <c r="H79" s="5" t="s">
@@ -7736,7 +7727,7 @@
       <c r="F84" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="G84" s="7">
+      <c r="G84" s="6">
         <v>30191</v>
       </c>
       <c r="H84" s="5" t="s">
@@ -7760,7 +7751,7 @@
         <v>53</v>
       </c>
       <c r="F85" s="5"/>
-      <c r="G85" s="7">
+      <c r="G85" s="6">
         <v>28096</v>
       </c>
       <c r="H85" s="5" t="s">
@@ -7784,7 +7775,7 @@
         <v>53</v>
       </c>
       <c r="F86" s="5"/>
-      <c r="G86" s="7">
+      <c r="G86" s="6">
         <v>33967</v>
       </c>
       <c r="H86" s="5" t="s">
@@ -7832,7 +7823,7 @@
         <v>24</v>
       </c>
       <c r="F88" s="5"/>
-      <c r="G88" s="7">
+      <c r="G88" s="6">
         <v>28865</v>
       </c>
       <c r="H88" s="5" t="s">
@@ -7856,7 +7847,7 @@
         <v>24</v>
       </c>
       <c r="F89" s="5"/>
-      <c r="G89" s="7">
+      <c r="G89" s="6">
         <v>35394</v>
       </c>
       <c r="H89" s="5" t="s">
@@ -7880,7 +7871,7 @@
         <v>24</v>
       </c>
       <c r="F90" s="5"/>
-      <c r="G90" s="7">
+      <c r="G90" s="6">
         <v>35875</v>
       </c>
       <c r="H90" s="5" t="s">
@@ -7952,7 +7943,7 @@
         <v>53</v>
       </c>
       <c r="F93" s="5"/>
-      <c r="G93" s="7">
+      <c r="G93" s="6">
         <v>36328</v>
       </c>
       <c r="H93" s="5" t="s">
@@ -7978,7 +7969,7 @@
       <c r="F94" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="G94" s="7">
+      <c r="G94" s="6">
         <v>29631</v>
       </c>
       <c r="H94" s="5" t="s">
@@ -8004,7 +7995,7 @@
       <c r="F95" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G95" s="7">
+      <c r="G95" s="6">
         <v>21129</v>
       </c>
       <c r="H95" s="5" t="s">
@@ -8078,7 +8069,7 @@
       <c r="F98" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G98" s="7">
+      <c r="G98" s="6">
         <v>31373</v>
       </c>
       <c r="H98" s="5" t="s">
@@ -8150,7 +8141,7 @@
         <v>24</v>
       </c>
       <c r="F101" s="5"/>
-      <c r="G101" s="7">
+      <c r="G101" s="6">
         <v>23509</v>
       </c>
       <c r="H101" s="5" t="s">
@@ -8200,7 +8191,7 @@
       <c r="F103" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G103" s="7">
+      <c r="G103" s="6">
         <v>20536</v>
       </c>
       <c r="H103" s="5" t="s">
@@ -8226,7 +8217,7 @@
       <c r="F104" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G104" s="7" t="s">
+      <c r="G104" s="6" t="s">
         <v>376</v>
       </c>
       <c r="H104" s="5" t="s">
@@ -8250,7 +8241,7 @@
         <v>53</v>
       </c>
       <c r="F105" s="5"/>
-      <c r="G105" s="7">
+      <c r="G105" s="6">
         <v>24699</v>
       </c>
       <c r="H105" s="5" t="s">
@@ -8276,7 +8267,7 @@
       <c r="F106" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G106" s="7">
+      <c r="G106" s="6">
         <v>32348</v>
       </c>
       <c r="H106" s="5" t="s">
@@ -8302,7 +8293,7 @@
       <c r="F107" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G107" s="7">
+      <c r="G107" s="6">
         <v>36137</v>
       </c>
       <c r="H107" s="5" t="s">
@@ -8328,7 +8319,7 @@
       <c r="F108" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G108" s="7">
+      <c r="G108" s="6">
         <v>28865</v>
       </c>
       <c r="H108" s="5" t="s">
@@ -8352,7 +8343,7 @@
         <v>53</v>
       </c>
       <c r="F109" s="5"/>
-      <c r="G109" s="7">
+      <c r="G109" s="6">
         <v>26395</v>
       </c>
       <c r="H109" s="5" t="s">
@@ -8378,7 +8369,7 @@
       <c r="F110" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G110" s="7">
+      <c r="G110" s="6">
         <v>28096</v>
       </c>
       <c r="H110" s="5" t="s">
@@ -8404,7 +8395,7 @@
       <c r="F111" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="G111" s="7">
+      <c r="G111" s="6">
         <v>30191</v>
       </c>
       <c r="H111" s="5" t="s">
@@ -8428,7 +8419,7 @@
         <v>24</v>
       </c>
       <c r="F112" s="5"/>
-      <c r="G112" s="7">
+      <c r="G112" s="6">
         <v>23509</v>
       </c>
       <c r="H112" s="5" t="s">
@@ -8452,7 +8443,7 @@
         <v>24</v>
       </c>
       <c r="F113" s="5"/>
-      <c r="G113" s="7">
+      <c r="G113" s="6">
         <v>31855</v>
       </c>
       <c r="H113" s="5" t="s">
@@ -8548,7 +8539,7 @@
         <v>53</v>
       </c>
       <c r="F117" s="5"/>
-      <c r="G117" s="7">
+      <c r="G117" s="6">
         <v>20536</v>
       </c>
       <c r="H117" s="5" t="s">
@@ -8572,7 +8563,7 @@
         <v>24</v>
       </c>
       <c r="F118" s="5"/>
-      <c r="G118" s="7">
+      <c r="G118" s="6">
         <v>21129</v>
       </c>
       <c r="H118" s="5" t="s">
@@ -8620,7 +8611,7 @@
         <v>24</v>
       </c>
       <c r="F120" s="5"/>
-      <c r="G120" s="7">
+      <c r="G120" s="6">
         <v>31855</v>
       </c>
       <c r="H120" s="5" t="s">
@@ -8716,7 +8707,7 @@
         <v>24</v>
       </c>
       <c r="F124" s="5"/>
-      <c r="G124" s="7">
+      <c r="G124" s="6">
         <v>20313</v>
       </c>
       <c r="H124" s="5" t="s">
@@ -8740,7 +8731,7 @@
         <v>24</v>
       </c>
       <c r="F125" s="5"/>
-      <c r="G125" s="7">
+      <c r="G125" s="6">
         <v>36137</v>
       </c>
       <c r="H125" s="5" t="s">
@@ -8766,7 +8757,7 @@
       <c r="F126" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G126" s="7">
+      <c r="G126" s="6">
         <v>32348</v>
       </c>
       <c r="H126" s="5" t="s">
@@ -8814,7 +8805,7 @@
         <v>24</v>
       </c>
       <c r="F128" s="5"/>
-      <c r="G128" s="7">
+      <c r="G128" s="6">
         <v>21366</v>
       </c>
       <c r="H128" s="5" t="s">
@@ -8888,7 +8879,7 @@
       <c r="F131" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="G131" s="7">
+      <c r="G131" s="6">
         <v>36328</v>
       </c>
       <c r="H131" s="5" t="s">
@@ -8960,7 +8951,7 @@
         <v>53</v>
       </c>
       <c r="F134" s="5"/>
-      <c r="G134" s="7">
+      <c r="G134" s="6">
         <v>33490</v>
       </c>
       <c r="H134" s="5" t="s">
@@ -9034,7 +9025,7 @@
       <c r="F137" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G137" s="7">
+      <c r="G137" s="6">
         <v>30191</v>
       </c>
       <c r="H137" s="5" t="s">
@@ -9058,7 +9049,7 @@
         <v>53</v>
       </c>
       <c r="F138" s="5"/>
-      <c r="G138" s="7">
+      <c r="G138" s="6">
         <v>35394</v>
       </c>
       <c r="H138" s="5" t="s">
@@ -9084,7 +9075,7 @@
       <c r="F139" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G139" s="7">
+      <c r="G139" s="6">
         <v>21129</v>
       </c>
       <c r="H139" s="5" t="s">
@@ -9108,7 +9099,7 @@
         <v>24</v>
       </c>
       <c r="F140" s="5"/>
-      <c r="G140" s="7">
+      <c r="G140" s="6">
         <v>26395</v>
       </c>
       <c r="H140" s="5" t="s">
@@ -9254,7 +9245,7 @@
       <c r="F146" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="G146" s="7">
+      <c r="G146" s="6">
         <v>23193</v>
       </c>
       <c r="H146" s="5" t="s">
@@ -9278,7 +9269,7 @@
         <v>53</v>
       </c>
       <c r="F147" s="5"/>
-      <c r="G147" s="7">
+      <c r="G147" s="6">
         <v>25121</v>
       </c>
       <c r="H147" s="5" t="s">
@@ -9302,7 +9293,7 @@
         <v>53</v>
       </c>
       <c r="F148" s="5"/>
-      <c r="G148" s="7">
+      <c r="G148" s="6">
         <v>20536</v>
       </c>
       <c r="H148" s="5" t="s">
@@ -9352,7 +9343,7 @@
       <c r="F150" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G150" s="7">
+      <c r="G150" s="6">
         <v>28640</v>
       </c>
       <c r="H150" s="5" t="s">
@@ -9378,7 +9369,7 @@
       <c r="F151" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G151" s="7">
+      <c r="G151" s="6">
         <v>34367</v>
       </c>
       <c r="H151" s="5" t="s">
@@ -9452,7 +9443,7 @@
       <c r="F154" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G154" s="7">
+      <c r="G154" s="6">
         <v>24699</v>
       </c>
       <c r="H154" s="5" t="s">
@@ -9572,7 +9563,7 @@
         <v>24</v>
       </c>
       <c r="F159" s="5"/>
-      <c r="G159" s="7">
+      <c r="G159" s="6">
         <v>20313</v>
       </c>
       <c r="H159" s="5" t="s">
@@ -9646,7 +9637,7 @@
       <c r="F162" s="5" t="s">
         <v>577</v>
       </c>
-      <c r="G162" s="7">
+      <c r="G162" s="6">
         <v>20313</v>
       </c>
       <c r="H162" s="5" t="s">
@@ -9718,7 +9709,7 @@
         <v>24</v>
       </c>
       <c r="F165" s="5"/>
-      <c r="G165" s="7">
+      <c r="G165" s="6">
         <v>23509</v>
       </c>
       <c r="H165" s="5" t="s">
@@ -9744,7 +9735,7 @@
       <c r="F166" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G166" s="7">
+      <c r="G166" s="6">
         <v>22562</v>
       </c>
       <c r="H166" s="5" t="s">
@@ -9792,7 +9783,7 @@
         <v>53</v>
       </c>
       <c r="F168" s="5"/>
-      <c r="G168" s="7">
+      <c r="G168" s="6">
         <v>35875</v>
       </c>
       <c r="H168" s="5" t="s">
@@ -9818,7 +9809,7 @@
       <c r="F169" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="G169" s="7">
+      <c r="G169" s="6">
         <v>34863</v>
       </c>
       <c r="H169" s="5" t="s">
@@ -9866,7 +9857,7 @@
         <v>24</v>
       </c>
       <c r="F171" s="5"/>
-      <c r="G171" s="7">
+      <c r="G171" s="6">
         <v>36137</v>
       </c>
       <c r="H171" s="5" t="s">
@@ -9962,7 +9953,7 @@
         <v>24</v>
       </c>
       <c r="F175" s="5"/>
-      <c r="G175" s="7">
+      <c r="G175" s="6">
         <v>30191</v>
       </c>
       <c r="H175" s="5" t="s">
@@ -10058,7 +10049,7 @@
         <v>53</v>
       </c>
       <c r="F179" s="5"/>
-      <c r="G179" s="7">
+      <c r="G179" s="6">
         <v>25121</v>
       </c>
       <c r="H179" s="5" t="s">
@@ -10106,7 +10097,7 @@
         <v>24</v>
       </c>
       <c r="F181" s="5"/>
-      <c r="G181" s="7">
+      <c r="G181" s="6">
         <v>22906</v>
       </c>
       <c r="H181" s="5" t="s">
@@ -10204,7 +10195,7 @@
       <c r="F185" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="G185" s="7">
+      <c r="G185" s="6">
         <v>28865</v>
       </c>
       <c r="H185" s="5" t="s">
@@ -10230,7 +10221,7 @@
       <c r="F186" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="G186" s="7">
+      <c r="G186" s="6">
         <v>24699</v>
       </c>
       <c r="H186" s="5" t="s">
@@ -10254,7 +10245,7 @@
         <v>24</v>
       </c>
       <c r="F187" s="5"/>
-      <c r="G187" s="7">
+      <c r="G187" s="6">
         <v>31373</v>
       </c>
       <c r="H187" s="5" t="s">
@@ -10280,7 +10271,7 @@
       <c r="F188" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G188" s="7">
+      <c r="G188" s="6">
         <v>31855</v>
       </c>
       <c r="H188" s="5" t="s">
@@ -10304,7 +10295,7 @@
         <v>24</v>
       </c>
       <c r="F189" s="5"/>
-      <c r="G189" s="7">
+      <c r="G189" s="6">
         <v>23509</v>
       </c>
       <c r="H189" s="5" t="s">
@@ -10328,7 +10319,7 @@
         <v>24</v>
       </c>
       <c r="F190" s="5"/>
-      <c r="G190" s="7">
+      <c r="G190" s="6">
         <v>21129</v>
       </c>
       <c r="H190" s="5" t="s">
@@ -10402,7 +10393,7 @@
       <c r="F193" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="G193" s="7">
+      <c r="G193" s="6">
         <v>37212</v>
       </c>
       <c r="H193" s="5" t="s">
@@ -10428,7 +10419,7 @@
       <c r="F194" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="G194" s="7">
+      <c r="G194" s="6">
         <v>26395</v>
       </c>
       <c r="H194" s="5" t="s">
@@ -10454,7 +10445,7 @@
       <c r="F195" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="G195" s="7">
+      <c r="G195" s="6">
         <v>20313</v>
       </c>
       <c r="H195" s="5" t="s">
@@ -10550,7 +10541,7 @@
         <v>24</v>
       </c>
       <c r="F199" s="5"/>
-      <c r="G199" s="7">
+      <c r="G199" s="6">
         <v>26251</v>
       </c>
       <c r="H199" s="5" t="s">
@@ -10576,7 +10567,7 @@
       <c r="F200" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G200" s="7">
+      <c r="G200" s="6">
         <v>22562</v>
       </c>
       <c r="H200" s="5" t="s">
@@ -10600,7 +10591,7 @@
         <v>24</v>
       </c>
       <c r="F201" s="5"/>
-      <c r="G201" s="7">
+      <c r="G201" s="6">
         <v>28640</v>
       </c>
       <c r="H201" s="5" t="s">
@@ -10648,7 +10639,7 @@
         <v>24</v>
       </c>
       <c r="F203" s="5"/>
-      <c r="G203" s="7">
+      <c r="G203" s="6">
         <v>32348</v>
       </c>
       <c r="H203" s="5" t="s">
@@ -10696,7 +10687,7 @@
         <v>24</v>
       </c>
       <c r="F205" s="5"/>
-      <c r="G205" s="7">
+      <c r="G205" s="6">
         <v>34185</v>
       </c>
       <c r="H205" s="5" t="s">
@@ -10746,7 +10737,7 @@
       <c r="F207" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="G207" s="7">
+      <c r="G207" s="6">
         <v>30191</v>
       </c>
       <c r="H207" s="5" t="s">
@@ -10770,7 +10761,7 @@
         <v>24</v>
       </c>
       <c r="F208" s="5"/>
-      <c r="G208" s="7">
+      <c r="G208" s="6">
         <v>36328</v>
       </c>
       <c r="H208" s="5" t="s">
@@ -10818,7 +10809,7 @@
         <v>24</v>
       </c>
       <c r="F210" s="5"/>
-      <c r="G210" s="7">
+      <c r="G210" s="6">
         <v>31855</v>
       </c>
       <c r="H210" s="5" t="s">
@@ -10842,7 +10833,7 @@
         <v>24</v>
       </c>
       <c r="F211" s="5"/>
-      <c r="G211" s="7">
+      <c r="G211" s="6">
         <v>21366</v>
       </c>
       <c r="H211" s="5" t="s">
@@ -10866,7 +10857,7 @@
         <v>24</v>
       </c>
       <c r="F212" s="5"/>
-      <c r="G212" s="7">
+      <c r="G212" s="6">
         <v>33011</v>
       </c>
       <c r="H212" s="5" t="s">
@@ -10892,7 +10883,7 @@
       <c r="F213" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="G213" s="7">
+      <c r="G213" s="6">
         <v>35436</v>
       </c>
       <c r="H213" s="5" t="s">
@@ -10940,7 +10931,7 @@
         <v>24</v>
       </c>
       <c r="F215" s="5"/>
-      <c r="G215" s="7">
+      <c r="G215" s="6">
         <v>23509</v>
       </c>
       <c r="H215" s="5" t="s">
@@ -10964,7 +10955,7 @@
         <v>24</v>
       </c>
       <c r="F216" s="5"/>
-      <c r="G216" s="7">
+      <c r="G216" s="6">
         <v>25372</v>
       </c>
       <c r="H216" s="5" t="s">
@@ -10990,7 +10981,7 @@
       <c r="F217" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="G217" s="7">
+      <c r="G217" s="6">
         <v>29631</v>
       </c>
       <c r="H217" s="5" t="s">
@@ -11014,7 +11005,7 @@
         <v>24</v>
       </c>
       <c r="F218" s="5"/>
-      <c r="G218" s="7">
+      <c r="G218" s="6">
         <v>33967</v>
       </c>
       <c r="H218" s="5" t="s">
@@ -11088,7 +11079,7 @@
       <c r="F221" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="G221" s="7">
+      <c r="G221" s="6">
         <v>21129</v>
       </c>
       <c r="H221" s="5" t="s">
@@ -11112,7 +11103,7 @@
         <v>24</v>
       </c>
       <c r="F222" s="5"/>
-      <c r="G222" s="7">
+      <c r="G222" s="6">
         <v>25121</v>
       </c>
       <c r="H222" s="5" t="s">
@@ -11136,7 +11127,7 @@
         <v>24</v>
       </c>
       <c r="F223" s="5"/>
-      <c r="G223" s="7">
+      <c r="G223" s="6">
         <v>30191</v>
       </c>
       <c r="H223" s="5" t="s">
@@ -11184,7 +11175,7 @@
         <v>24</v>
       </c>
       <c r="F225" s="5"/>
-      <c r="G225" s="7">
+      <c r="G225" s="6">
         <v>35436</v>
       </c>
       <c r="H225" s="5" t="s">
@@ -11210,7 +11201,7 @@
       <c r="F226" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="G226" s="7">
+      <c r="G226" s="6">
         <v>29409</v>
       </c>
       <c r="H226" s="5" t="s">
@@ -11258,7 +11249,7 @@
         <v>24</v>
       </c>
       <c r="F228" s="5"/>
-      <c r="G228" s="7">
+      <c r="G228" s="6">
         <v>36328</v>
       </c>
       <c r="H228" s="5" t="s">
@@ -11306,7 +11297,7 @@
         <v>24</v>
       </c>
       <c r="F230" s="5"/>
-      <c r="G230" s="7">
+      <c r="G230" s="6">
         <v>34863</v>
       </c>
       <c r="H230" s="5" t="s">
@@ -11332,7 +11323,7 @@
       <c r="F231" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="G231" s="7">
+      <c r="G231" s="6">
         <v>34185</v>
       </c>
       <c r="H231" s="5" t="s">
@@ -11428,7 +11419,7 @@
         <v>53</v>
       </c>
       <c r="F235" s="5"/>
-      <c r="G235" s="7">
+      <c r="G235" s="6">
         <v>21366</v>
       </c>
       <c r="H235" s="5" t="s">
@@ -11454,7 +11445,7 @@
       <c r="F236" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="G236" s="7">
+      <c r="G236" s="6">
         <v>36356</v>
       </c>
       <c r="H236" s="5" t="s">
@@ -11526,7 +11517,7 @@
         <v>53</v>
       </c>
       <c r="F239" s="5"/>
-      <c r="G239" s="7">
+      <c r="G239" s="6">
         <v>25372</v>
       </c>
       <c r="H239" s="5" t="s">
@@ -11624,7 +11615,7 @@
       <c r="F243" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="G243" s="7">
+      <c r="G243" s="6">
         <v>35875</v>
       </c>
       <c r="H243" s="5" t="s">
@@ -11698,7 +11689,7 @@
       <c r="F246" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="G246" s="7">
+      <c r="G246" s="6">
         <v>22906</v>
       </c>
       <c r="H246" s="5" t="s">
@@ -11748,7 +11739,7 @@
       <c r="F248" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G248" s="7">
+      <c r="G248" s="6">
         <v>36328</v>
       </c>
       <c r="H248" s="5" t="s">
@@ -11916,7 +11907,7 @@
         <v>24</v>
       </c>
       <c r="F255" s="5"/>
-      <c r="G255" s="7">
+      <c r="G255" s="6">
         <v>34185</v>
       </c>
       <c r="H255" s="5" t="s">
@@ -11964,7 +11955,7 @@
         <v>24</v>
       </c>
       <c r="F257" s="5"/>
-      <c r="G257" s="7">
+      <c r="G257" s="6">
         <v>31855</v>
       </c>
       <c r="H257" s="5" t="s">
@@ -11988,7 +11979,7 @@
         <v>24</v>
       </c>
       <c r="F258" s="5"/>
-      <c r="G258" s="7">
+      <c r="G258" s="6">
         <v>25372</v>
       </c>
       <c r="H258" s="5" t="s">
@@ -12038,7 +12029,7 @@
       <c r="F260" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="G260" s="7">
+      <c r="G260" s="6">
         <v>30191</v>
       </c>
       <c r="H260" s="5" t="s">
@@ -12064,7 +12055,7 @@
       <c r="F261" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="G261" s="7">
+      <c r="G261" s="6">
         <v>28640</v>
       </c>
       <c r="H261" s="5" t="s">
@@ -12112,7 +12103,7 @@
         <v>24</v>
       </c>
       <c r="F263" s="5"/>
-      <c r="G263" s="7">
+      <c r="G263" s="6">
         <v>35394</v>
       </c>
       <c r="H263" s="5" t="s">
@@ -12184,7 +12175,7 @@
         <v>24</v>
       </c>
       <c r="F266" s="5"/>
-      <c r="G266" s="7">
+      <c r="G266" s="6">
         <v>20313</v>
       </c>
       <c r="H266" s="5" t="s">
@@ -12234,7 +12225,7 @@
       <c r="F268" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="G268" s="7">
+      <c r="G268" s="6">
         <v>20313</v>
       </c>
       <c r="H268" s="5" t="s">
@@ -12260,7 +12251,7 @@
       <c r="F269" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G269" s="7">
+      <c r="G269" s="6">
         <v>26395</v>
       </c>
       <c r="H269" s="5" t="s">
@@ -12308,7 +12299,7 @@
         <v>24</v>
       </c>
       <c r="F271" s="5"/>
-      <c r="G271" s="7">
+      <c r="G271" s="6">
         <v>28865</v>
       </c>
       <c r="H271" s="5" t="s">
@@ -12430,7 +12421,7 @@
       <c r="F276" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="G276" s="7">
+      <c r="G276" s="6">
         <v>25121</v>
       </c>
       <c r="H276" s="5" t="s">
@@ -12526,7 +12517,7 @@
         <v>24</v>
       </c>
       <c r="F280" s="5"/>
-      <c r="G280" s="7">
+      <c r="G280" s="6">
         <v>28640</v>
       </c>
       <c r="H280" s="5" t="s">
@@ -12550,7 +12541,7 @@
         <v>24</v>
       </c>
       <c r="F281" s="5"/>
-      <c r="G281" s="7">
+      <c r="G281" s="6">
         <v>35394</v>
       </c>
       <c r="H281" s="5" t="s">
@@ -12622,7 +12613,7 @@
         <v>24</v>
       </c>
       <c r="F284" s="5"/>
-      <c r="G284" s="7">
+      <c r="G284" s="6">
         <v>35436</v>
       </c>
       <c r="H284" s="5" t="s">
@@ -12646,7 +12637,7 @@
         <v>24</v>
       </c>
       <c r="F285" s="5"/>
-      <c r="G285" s="7">
+      <c r="G285" s="6">
         <v>20313</v>
       </c>
       <c r="H285" s="5" t="s">
@@ -12694,7 +12685,7 @@
         <v>24</v>
       </c>
       <c r="F287" s="5"/>
-      <c r="G287" s="7">
+      <c r="G287" s="6">
         <v>33490</v>
       </c>
       <c r="H287" s="5" t="s">
@@ -12718,7 +12709,7 @@
         <v>24</v>
       </c>
       <c r="F288" s="5"/>
-      <c r="G288" s="7">
+      <c r="G288" s="6">
         <v>36276</v>
       </c>
       <c r="H288" s="5" t="s">
@@ -12792,7 +12783,7 @@
       <c r="F291" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="G291" s="7">
+      <c r="G291" s="6">
         <v>21654</v>
       </c>
       <c r="H291" s="5" t="s">
@@ -12840,7 +12831,7 @@
         <v>24</v>
       </c>
       <c r="F293" s="5"/>
-      <c r="G293" s="7">
+      <c r="G293" s="6">
         <v>34367</v>
       </c>
       <c r="H293" s="5" t="s">
@@ -12912,7 +12903,7 @@
         <v>24</v>
       </c>
       <c r="F296" s="5"/>
-      <c r="G296" s="7">
+      <c r="G296" s="6">
         <v>34185</v>
       </c>
       <c r="H296" s="5" t="s">
@@ -12938,7 +12929,7 @@
       <c r="F297" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="G297" s="7">
+      <c r="G297" s="6">
         <v>25121</v>
       </c>
       <c r="H297" s="5" t="s">
@@ -12964,7 +12955,7 @@
       <c r="F298" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="G298" s="7">
+      <c r="G298" s="6">
         <v>36328</v>
       </c>
       <c r="H298" s="5" t="s">
@@ -12988,7 +12979,7 @@
         <v>24</v>
       </c>
       <c r="F299" s="5"/>
-      <c r="G299" s="7">
+      <c r="G299" s="6">
         <v>26251</v>
       </c>
       <c r="H299" s="5" t="s">
@@ -13014,7 +13005,7 @@
       <c r="F300" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="G300" s="7">
+      <c r="G300" s="6">
         <v>28865</v>
       </c>
       <c r="H300" s="5" t="s">
@@ -13038,7 +13029,7 @@
         <v>24</v>
       </c>
       <c r="F301" s="5"/>
-      <c r="G301" s="7">
+      <c r="G301" s="6">
         <v>25372</v>
       </c>
       <c r="H301" s="5" t="s">
@@ -13158,7 +13149,7 @@
         <v>24</v>
       </c>
       <c r="F306" s="5"/>
-      <c r="G306" s="7">
+      <c r="G306" s="6">
         <v>34367</v>
       </c>
       <c r="H306" s="5" t="s">
@@ -13182,7 +13173,7 @@
         <v>24</v>
       </c>
       <c r="F307" s="5"/>
-      <c r="G307" s="7">
+      <c r="G307" s="6">
         <v>28640</v>
       </c>
       <c r="H307" s="5" t="s">
@@ -13206,7 +13197,7 @@
         <v>24</v>
       </c>
       <c r="F308" s="5"/>
-      <c r="G308" s="7">
+      <c r="G308" s="6">
         <v>32812</v>
       </c>
       <c r="H308" s="5" t="s">
@@ -13328,7 +13319,7 @@
       <c r="F313" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G313" s="7">
+      <c r="G313" s="6">
         <v>31855</v>
       </c>
       <c r="H313" s="5" t="s">
@@ -13400,7 +13391,7 @@
         <v>24</v>
       </c>
       <c r="F316" s="5"/>
-      <c r="G316" s="7">
+      <c r="G316" s="6">
         <v>35875</v>
       </c>
       <c r="H316" s="5" t="s">
@@ -13450,7 +13441,7 @@
       <c r="F318" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="G318" s="7">
+      <c r="G318" s="6">
         <v>34863</v>
       </c>
       <c r="H318" s="5" t="s">
@@ -13570,7 +13561,7 @@
         <v>24</v>
       </c>
       <c r="F323" s="5"/>
-      <c r="G323" s="7">
+      <c r="G323" s="6">
         <v>32812</v>
       </c>
       <c r="H323" s="5" t="s">
@@ -13644,7 +13635,7 @@
       <c r="F326" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G326" s="7">
+      <c r="G326" s="6">
         <v>28865</v>
       </c>
       <c r="H326" s="5" t="s">
@@ -13668,7 +13659,7 @@
         <v>24</v>
       </c>
       <c r="F327" s="5"/>
-      <c r="G327" s="7">
+      <c r="G327" s="6">
         <v>30775</v>
       </c>
       <c r="H327" s="5" t="s">
@@ -13740,7 +13731,7 @@
         <v>24</v>
       </c>
       <c r="F330" s="5"/>
-      <c r="G330" s="7">
+      <c r="G330" s="6">
         <v>35436</v>
       </c>
       <c r="H330" s="5" t="s">
@@ -13862,7 +13853,7 @@
       <c r="F335" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="G335" s="7">
+      <c r="G335" s="6">
         <v>28640</v>
       </c>
       <c r="H335" s="5" t="s">
@@ -13888,7 +13879,7 @@
       <c r="F336" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G336" s="7">
+      <c r="G336" s="6">
         <v>21654</v>
       </c>
       <c r="H336" s="5" t="s">
@@ -13960,7 +13951,7 @@
         <v>24</v>
       </c>
       <c r="F339" s="5"/>
-      <c r="G339" s="7">
+      <c r="G339" s="6">
         <v>22562</v>
       </c>
       <c r="H339" s="5" t="s">
@@ -13984,7 +13975,7 @@
         <v>24</v>
       </c>
       <c r="F340" s="5"/>
-      <c r="G340" s="7">
+      <c r="G340" s="6">
         <v>26251</v>
       </c>
       <c r="H340" s="5" t="s">
@@ -14080,7 +14071,7 @@
         <v>24</v>
       </c>
       <c r="F344" s="5"/>
-      <c r="G344" s="7">
+      <c r="G344" s="6">
         <v>34185</v>
       </c>
       <c r="H344" s="5" t="s">
@@ -14106,7 +14097,7 @@
       <c r="F345" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G345" s="7">
+      <c r="G345" s="6">
         <v>28640</v>
       </c>
       <c r="H345" s="5" t="s">
@@ -14180,7 +14171,7 @@
       <c r="F348" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G348" s="7">
+      <c r="G348" s="6">
         <v>26874</v>
       </c>
       <c r="H348" s="5" t="s">
@@ -14206,7 +14197,7 @@
       <c r="F349" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="G349" s="7">
+      <c r="G349" s="6">
         <v>36276</v>
       </c>
       <c r="H349" s="5" t="s">
@@ -14280,7 +14271,7 @@
       <c r="F352" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G352" s="7">
+      <c r="G352" s="6">
         <v>36328</v>
       </c>
       <c r="H352" s="5" t="s">
@@ -14352,7 +14343,7 @@
         <v>24</v>
       </c>
       <c r="F355" s="5"/>
-      <c r="G355" s="7">
+      <c r="G355" s="6">
         <v>21129</v>
       </c>
       <c r="H355" s="5" t="s">
@@ -14378,7 +14369,7 @@
       <c r="F356" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="G356" s="7">
+      <c r="G356" s="6">
         <v>22906</v>
       </c>
       <c r="H356" s="5" t="s">
@@ -14402,7 +14393,7 @@
         <v>24</v>
       </c>
       <c r="F357" s="5"/>
-      <c r="G357" s="7">
+      <c r="G357" s="6">
         <v>20313</v>
       </c>
       <c r="H357" s="5" t="s">
@@ -14474,7 +14465,7 @@
         <v>24</v>
       </c>
       <c r="F360" s="5"/>
-      <c r="G360" s="7">
+      <c r="G360" s="6">
         <v>28297</v>
       </c>
       <c r="H360" s="5" t="s">
@@ -14524,7 +14515,7 @@
       <c r="F362" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G362" s="7">
+      <c r="G362" s="6">
         <v>30775</v>
       </c>
       <c r="H362" s="5" t="s">
@@ -14620,7 +14611,7 @@
         <v>24</v>
       </c>
       <c r="F366" s="5"/>
-      <c r="G366" s="7">
+      <c r="G366" s="6">
         <v>35436</v>
       </c>
       <c r="H366" s="5" t="s">
@@ -14646,7 +14637,7 @@
       <c r="F367" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="G367" s="7">
+      <c r="G367" s="6">
         <v>22906</v>
       </c>
       <c r="H367" s="5" t="s">
@@ -14670,7 +14661,7 @@
         <v>24</v>
       </c>
       <c r="F368" s="5"/>
-      <c r="G368" s="7">
+      <c r="G368" s="6">
         <v>25372</v>
       </c>
       <c r="H368" s="5" t="s">
@@ -14696,7 +14687,7 @@
       <c r="F369" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="G369" s="7">
+      <c r="G369" s="6">
         <v>35875</v>
       </c>
       <c r="H369" s="5" t="s">
@@ -14744,7 +14735,7 @@
         <v>24</v>
       </c>
       <c r="F371" s="5"/>
-      <c r="G371" s="7">
+      <c r="G371" s="6">
         <v>26874</v>
       </c>
       <c r="H371" s="5" t="s">
@@ -14890,7 +14881,7 @@
       <c r="F377" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="G377" s="7">
+      <c r="G377" s="6">
         <v>36356</v>
       </c>
       <c r="H377" s="5" t="s">
@@ -14938,7 +14929,7 @@
         <v>24</v>
       </c>
       <c r="F379" s="5"/>
-      <c r="G379" s="7">
+      <c r="G379" s="6">
         <v>36356</v>
       </c>
       <c r="H379" s="5" t="s">
@@ -14988,7 +14979,7 @@
       <c r="F381" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G381" s="7">
+      <c r="G381" s="6">
         <v>36356</v>
       </c>
       <c r="H381" s="5" t="s">
@@ -15012,7 +15003,7 @@
         <v>24</v>
       </c>
       <c r="F382" s="5"/>
-      <c r="G382" s="7">
+      <c r="G382" s="6">
         <v>36328</v>
       </c>
       <c r="H382" s="5" t="s">
@@ -15060,7 +15051,7 @@
         <v>24</v>
       </c>
       <c r="F384" s="5"/>
-      <c r="G384" s="7">
+      <c r="G384" s="6">
         <v>25372</v>
       </c>
       <c r="H384" s="5" t="s">
@@ -15180,7 +15171,7 @@
         <v>24</v>
       </c>
       <c r="F389" s="5"/>
-      <c r="G389" s="7">
+      <c r="G389" s="6">
         <v>36276</v>
       </c>
       <c r="H389" s="5" t="s">
@@ -15252,7 +15243,7 @@
         <v>24</v>
       </c>
       <c r="F392" s="5"/>
-      <c r="G392" s="7">
+      <c r="G392" s="6">
         <v>20313</v>
       </c>
       <c r="H392" s="5" t="s">
@@ -15300,7 +15291,7 @@
         <v>24</v>
       </c>
       <c r="F394" s="5"/>
-      <c r="G394" s="7">
+      <c r="G394" s="6">
         <v>25626</v>
       </c>
       <c r="H394" s="5" t="s">
@@ -15348,7 +15339,7 @@
         <v>24</v>
       </c>
       <c r="F396" s="5"/>
-      <c r="G396" s="7">
+      <c r="G396" s="6">
         <v>34185</v>
       </c>
       <c r="H396" s="5" t="s">
@@ -15374,7 +15365,7 @@
       <c r="F397" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G397" s="7">
+      <c r="G397" s="6">
         <v>29631</v>
       </c>
       <c r="H397" s="5" t="s">
@@ -15398,7 +15389,7 @@
         <v>24</v>
       </c>
       <c r="F398" s="5"/>
-      <c r="G398" s="7">
+      <c r="G398" s="6">
         <v>35733</v>
       </c>
       <c r="H398" s="5" t="s">
@@ -15446,7 +15437,7 @@
         <v>24</v>
       </c>
       <c r="F400" s="5"/>
-      <c r="G400" s="7">
+      <c r="G400" s="6">
         <v>35436</v>
       </c>
       <c r="H400" s="5" t="s">
@@ -15520,7 +15511,7 @@
       <c r="F403" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G403" s="7">
+      <c r="G403" s="6">
         <v>26395</v>
       </c>
       <c r="H403" s="5" t="s">
@@ -15594,7 +15585,7 @@
       <c r="F406" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="G406" s="7">
+      <c r="G406" s="6">
         <v>32812</v>
       </c>
       <c r="H406" s="5" t="s">
@@ -15618,7 +15609,7 @@
         <v>24</v>
       </c>
       <c r="F407" s="5"/>
-      <c r="G407" s="7">
+      <c r="G407" s="6">
         <v>31572</v>
       </c>
       <c r="H407" s="5" t="s">
@@ -15666,7 +15657,7 @@
         <v>24</v>
       </c>
       <c r="F409" s="5"/>
-      <c r="G409" s="7">
+      <c r="G409" s="6">
         <v>26874</v>
       </c>
       <c r="H409" s="5" t="s">
@@ -15716,7 +15707,7 @@
       <c r="F411" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G411" s="7">
+      <c r="G411" s="6">
         <v>22906</v>
       </c>
       <c r="H411" s="5" t="s">
@@ -15740,7 +15731,7 @@
         <v>24</v>
       </c>
       <c r="F412" s="5"/>
-      <c r="G412" s="7">
+      <c r="G412" s="6">
         <v>28297</v>
       </c>
       <c r="H412" s="5" t="s">
@@ -15764,7 +15755,7 @@
         <v>24</v>
       </c>
       <c r="F413" s="5"/>
-      <c r="G413" s="7">
+      <c r="G413" s="6">
         <v>30775</v>
       </c>
       <c r="H413" s="5" t="s">
@@ -15788,7 +15779,7 @@
         <v>24</v>
       </c>
       <c r="F414" s="5"/>
-      <c r="G414" s="7">
+      <c r="G414" s="6">
         <v>31572</v>
       </c>
       <c r="H414" s="5" t="s">
@@ -15812,7 +15803,7 @@
         <v>24</v>
       </c>
       <c r="F415" s="5"/>
-      <c r="G415" s="7">
+      <c r="G415" s="6">
         <v>21654</v>
       </c>
       <c r="H415" s="5" t="s">
@@ -15860,7 +15851,7 @@
         <v>24</v>
       </c>
       <c r="F417" s="5"/>
-      <c r="G417" s="7">
+      <c r="G417" s="6">
         <v>28297</v>
       </c>
       <c r="H417" s="5" t="s">
@@ -15910,7 +15901,7 @@
       <c r="F419" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G419" s="7">
+      <c r="G419" s="6">
         <v>35733</v>
       </c>
       <c r="H419" s="5" t="s">
@@ -15958,7 +15949,7 @@
         <v>24</v>
       </c>
       <c r="F421" s="5"/>
-      <c r="G421" s="7">
+      <c r="G421" s="6">
         <v>36276</v>
       </c>
       <c r="H421" s="5" t="s">
@@ -16078,7 +16069,7 @@
         <v>24</v>
       </c>
       <c r="F426" s="5"/>
-      <c r="G426" s="7">
+      <c r="G426" s="6">
         <v>32812</v>
       </c>
       <c r="H426" s="5" t="s">
@@ -16128,7 +16119,7 @@
       <c r="F428" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G428" s="7">
+      <c r="G428" s="6">
         <v>36356</v>
       </c>
       <c r="H428" s="5" t="s">
@@ -16152,7 +16143,7 @@
         <v>24</v>
       </c>
       <c r="F429" s="5"/>
-      <c r="G429" s="7">
+      <c r="G429" s="6">
         <v>24169</v>
       </c>
       <c r="H429" s="5" t="s">
@@ -16176,7 +16167,7 @@
         <v>24</v>
       </c>
       <c r="F430" s="5"/>
-      <c r="G430" s="7">
+      <c r="G430" s="6">
         <v>26874</v>
       </c>
       <c r="H430" s="5" t="s">
@@ -16200,7 +16191,7 @@
         <v>24</v>
       </c>
       <c r="F431" s="5"/>
-      <c r="G431" s="7">
+      <c r="G431" s="6">
         <v>26251</v>
       </c>
       <c r="H431" s="5" t="s">
@@ -16248,7 +16239,7 @@
         <v>24</v>
       </c>
       <c r="F433" s="5"/>
-      <c r="G433" s="7">
+      <c r="G433" s="6">
         <v>21654</v>
       </c>
       <c r="H433" s="5" t="s">
@@ -16296,7 +16287,7 @@
         <v>24</v>
       </c>
       <c r="F435" s="5"/>
-      <c r="G435" s="7">
+      <c r="G435" s="6">
         <v>22906</v>
       </c>
       <c r="H435" s="5" t="s">
@@ -16320,7 +16311,7 @@
         <v>24</v>
       </c>
       <c r="F436" s="5"/>
-      <c r="G436" s="7">
+      <c r="G436" s="6">
         <v>25372</v>
       </c>
       <c r="H436" s="5" t="s">
@@ -16346,7 +16337,7 @@
       <c r="F437" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G437" s="7">
+      <c r="G437" s="6">
         <v>30775</v>
       </c>
       <c r="H437" s="5" t="s">
@@ -16418,7 +16409,7 @@
         <v>24</v>
       </c>
       <c r="F440" s="5"/>
-      <c r="G440" s="7">
+      <c r="G440" s="6">
         <v>33967</v>
       </c>
       <c r="H440" s="5" t="s">
@@ -16442,7 +16433,7 @@
         <v>24</v>
       </c>
       <c r="F441" s="5"/>
-      <c r="G441" s="7">
+      <c r="G441" s="6">
         <v>27277</v>
       </c>
       <c r="H441" s="5" t="s">
@@ -16490,7 +16481,7 @@
         <v>24</v>
       </c>
       <c r="F443" s="5"/>
-      <c r="G443" s="7">
+      <c r="G443" s="6">
         <v>33967</v>
       </c>
       <c r="H443" s="5" t="s">
@@ -16538,7 +16529,7 @@
         <v>24</v>
       </c>
       <c r="F445" s="5"/>
-      <c r="G445" s="7">
+      <c r="G445" s="6">
         <v>35733</v>
       </c>
       <c r="H445" s="5" t="s">
@@ -16564,7 +16555,7 @@
       <c r="F446" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G446" s="7">
+      <c r="G446" s="6">
         <v>21654</v>
       </c>
       <c r="H446" s="5" t="s">
@@ -16662,7 +16653,7 @@
       <c r="F450" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="G450" s="7">
+      <c r="G450" s="6">
         <v>32812</v>
       </c>
       <c r="H450" s="5" t="s">
@@ -16686,7 +16677,7 @@
         <v>24</v>
       </c>
       <c r="F451" s="5"/>
-      <c r="G451" s="7">
+      <c r="G451" s="6">
         <v>27277</v>
       </c>
       <c r="H451" s="5" t="s">
@@ -16782,7 +16773,7 @@
         <v>24</v>
       </c>
       <c r="F455" s="5"/>
-      <c r="G455" s="7">
+      <c r="G455" s="6">
         <v>33967</v>
       </c>
       <c r="H455" s="5" t="s">
@@ -16806,7 +16797,7 @@
         <v>24</v>
       </c>
       <c r="F456" s="5"/>
-      <c r="G456" s="7">
+      <c r="G456" s="6">
         <v>35436</v>
       </c>
       <c r="H456" s="5" t="s">
@@ -16854,7 +16845,7 @@
         <v>24</v>
       </c>
       <c r="F458" s="5"/>
-      <c r="G458" s="7">
+      <c r="G458" s="6">
         <v>22906</v>
       </c>
       <c r="H458" s="5" t="s">
@@ -16878,7 +16869,7 @@
         <v>24</v>
       </c>
       <c r="F459" s="5"/>
-      <c r="G459" s="7">
+      <c r="G459" s="6">
         <v>33967</v>
       </c>
       <c r="H459" s="5" t="s">
@@ -16904,7 +16895,7 @@
       <c r="F460" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G460" s="7">
+      <c r="G460" s="6">
         <v>33490</v>
       </c>
       <c r="H460" s="5" t="s">
@@ -16930,7 +16921,7 @@
       <c r="F461" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="G461" s="7">
+      <c r="G461" s="6">
         <v>26874</v>
       </c>
       <c r="H461" s="5" t="s">
@@ -16956,7 +16947,7 @@
       <c r="F462" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="G462" s="7">
+      <c r="G462" s="6">
         <v>28297</v>
       </c>
       <c r="H462" s="5" t="s">
@@ -17004,7 +16995,7 @@
         <v>24</v>
       </c>
       <c r="F464" s="5"/>
-      <c r="G464" s="7">
+      <c r="G464" s="6">
         <v>35733</v>
       </c>
       <c r="H464" s="5" t="s">
@@ -17028,7 +17019,7 @@
         <v>24</v>
       </c>
       <c r="F465" s="5"/>
-      <c r="G465" s="7">
+      <c r="G465" s="6">
         <v>36328</v>
       </c>
       <c r="H465" s="5" t="s">
@@ -17052,7 +17043,7 @@
         <v>24</v>
       </c>
       <c r="F466" s="5"/>
-      <c r="G466" s="7">
+      <c r="G466" s="6">
         <v>31572</v>
       </c>
       <c r="H466" s="5" t="s">
@@ -17076,7 +17067,7 @@
         <v>24</v>
       </c>
       <c r="F467" s="5"/>
-      <c r="G467" s="7">
+      <c r="G467" s="6">
         <v>21654</v>
       </c>
       <c r="H467" s="5" t="s">
@@ -17124,7 +17115,7 @@
         <v>24</v>
       </c>
       <c r="F469" s="5"/>
-      <c r="G469" s="7">
+      <c r="G469" s="6">
         <v>32812</v>
       </c>
       <c r="H469" s="5" t="s">
@@ -17150,7 +17141,7 @@
       <c r="F470" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G470" s="7">
+      <c r="G470" s="6">
         <v>36328</v>
       </c>
       <c r="H470" s="5" t="s">
@@ -17296,7 +17287,7 @@
       <c r="F476" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="G476" s="7">
+      <c r="G476" s="6">
         <v>36328</v>
       </c>
       <c r="H476" s="5" t="s">
@@ -17322,7 +17313,7 @@
       <c r="F477" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="G477" s="7">
+      <c r="G477" s="6">
         <v>27277</v>
       </c>
       <c r="H477" s="5" t="s">
@@ -17346,7 +17337,7 @@
         <v>24</v>
       </c>
       <c r="F478" s="5"/>
-      <c r="G478" s="7">
+      <c r="G478" s="6">
         <v>32812</v>
       </c>
       <c r="H478" s="5" t="s">
@@ -17370,7 +17361,7 @@
         <v>24</v>
       </c>
       <c r="F479" s="5"/>
-      <c r="G479" s="7">
+      <c r="G479" s="6">
         <v>30775</v>
       </c>
       <c r="H479" s="5" t="s">
@@ -17442,7 +17433,7 @@
         <v>24</v>
       </c>
       <c r="F482" s="5"/>
-      <c r="G482" s="7">
+      <c r="G482" s="6">
         <v>21654</v>
       </c>
       <c r="H482" s="5" t="s">
@@ -17490,7 +17481,7 @@
         <v>24</v>
       </c>
       <c r="F484" s="5"/>
-      <c r="G484" s="7">
+      <c r="G484" s="6">
         <v>35733</v>
       </c>
       <c r="H484" s="5" t="s">
@@ -17516,7 +17507,7 @@
       <c r="F485" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G485" s="7">
+      <c r="G485" s="6">
         <v>31572</v>
       </c>
       <c r="H485" s="5" t="s">
@@ -17542,7 +17533,7 @@
       <c r="F486" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G486" s="7">
+      <c r="G486" s="6">
         <v>26874</v>
       </c>
       <c r="H486" s="5" t="s">
@@ -17566,7 +17557,7 @@
         <v>24</v>
       </c>
       <c r="F487" s="5"/>
-      <c r="G487" s="7">
+      <c r="G487" s="6">
         <v>22562</v>
       </c>
       <c r="H487" s="5" t="s">
@@ -17590,7 +17581,7 @@
         <v>24</v>
       </c>
       <c r="F488" s="5"/>
-      <c r="G488" s="7">
+      <c r="G488" s="6">
         <v>25121</v>
       </c>
       <c r="H488" s="5" t="s">
@@ -17638,7 +17629,7 @@
         <v>24</v>
       </c>
       <c r="F490" s="5"/>
-      <c r="G490" s="7">
+      <c r="G490" s="6">
         <v>36276</v>
       </c>
       <c r="H490" s="5" t="s">
@@ -17686,7 +17677,7 @@
         <v>24</v>
       </c>
       <c r="F492" s="5"/>
-      <c r="G492" s="7">
+      <c r="G492" s="6">
         <v>35436</v>
       </c>
       <c r="H492" s="5" t="s">
@@ -17710,7 +17701,7 @@
         <v>24</v>
       </c>
       <c r="F493" s="5"/>
-      <c r="G493" s="7">
+      <c r="G493" s="6">
         <v>33490</v>
       </c>
       <c r="H493" s="5" t="s">
@@ -17734,7 +17725,7 @@
         <v>24</v>
       </c>
       <c r="F494" s="5"/>
-      <c r="G494" s="7">
+      <c r="G494" s="6">
         <v>24169</v>
       </c>
       <c r="H494" s="5" t="s">
@@ -17758,7 +17749,7 @@
         <v>24</v>
       </c>
       <c r="F495" s="5"/>
-      <c r="G495" s="7">
+      <c r="G495" s="6">
         <v>29409</v>
       </c>
       <c r="H495" s="5" t="s">
@@ -17784,7 +17775,7 @@
       <c r="F496" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="G496" s="7">
+      <c r="G496" s="6">
         <v>25626</v>
       </c>
       <c r="H496" s="5" t="s">
@@ -17906,7 +17897,7 @@
       <c r="F501" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="G501" s="7">
+      <c r="G501" s="6">
         <v>27469</v>
       </c>
       <c r="H501" s="5" t="s">

</xml_diff>